<commit_message>
Add initial support for JK BMS MQQT Data Retrieval (Data obtained from JK BMS using https://github.com/syssi/esphome-jk-bms via BLE)
</commit_message>
<xml_diff>
--- a/strategy/2024-01-14.xlsx
+++ b/strategy/2024-01-14.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,7 +445,7 @@
         <v>184</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>50</v>
@@ -474,7 +474,7 @@
         <v>182</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="H4" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -504,7 +504,7 @@
         <v>183</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="H5" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -534,7 +534,7 @@
         <v>184</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="H6" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -564,7 +564,7 @@
         <v>185</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -594,7 +594,7 @@
         <v>185</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="H8" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1074,7 +1074,7 @@
         <v>225</v>
       </c>
       <c r="G24" s="1" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1104,7 +1104,7 @@
         <v>222</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">$H$3</f>
@@ -1134,7 +1134,7 @@
         <v>215</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="H26" s="1" t="n">
         <f aca="false">$H$3</f>

</xml_diff>